<commit_message>
Changed font to calibiri
</commit_message>
<xml_diff>
--- a/Past Paper Tracker Template.xlsx
+++ b/Past Paper Tracker Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ray\Downloads\RAmjad's Notes &amp; Flashcards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\a-level-resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A146DE-62DF-4DCD-90A7-59DA60393C37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D49BA0-55FD-4C6C-90A4-37AB4853BD42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -94,7 +96,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmm\ dd"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -102,21 +104,26 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Proxima Nova"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
-      <name val="Proxima Nova"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Proxima Nova"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -279,60 +286,61 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="1" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="10" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="1" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="1" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -654,12 +662,15 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4:Q5"/>
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="14.44140625" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" customHeight="1">
+    <row r="1" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -679,239 +690,239 @@
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
     </row>
-    <row r="2" spans="1:18" ht="15.75" customHeight="1">
+    <row r="2" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="13" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="M2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="N2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="13" t="s">
+      <c r="O2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="13" t="s">
+      <c r="P2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="13" t="s">
+      <c r="Q2" s="5" t="s">
         <v>14</v>
       </c>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:18" ht="15.75" customHeight="1">
+    <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" ht="15.75" customHeight="1">
+    <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="4">
+      <c r="C4" s="4"/>
+      <c r="D4" s="9">
         <v>0.5</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="17"/>
-    </row>
-    <row r="5" spans="1:18" ht="15.75" customHeight="1">
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="10"/>
+    </row>
+    <row r="5" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="18"/>
-    </row>
-    <row r="6" spans="1:18" ht="15.75" customHeight="1">
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="14"/>
+    </row>
+    <row r="6" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="16"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="17"/>
-    </row>
-    <row r="7" spans="1:18" ht="15.75" customHeight="1">
+      <c r="D6" s="17"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="10"/>
+    </row>
+    <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="23"/>
-    </row>
-    <row r="8" spans="1:18" ht="15.75" customHeight="1">
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="18"/>
+    </row>
+    <row r="8" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="17"/>
-    </row>
-    <row r="9" spans="1:18" ht="15.75" customHeight="1">
+      <c r="C8" s="4"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="10"/>
+    </row>
+    <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="23"/>
-    </row>
-    <row r="10" spans="1:18" ht="15.75" customHeight="1">
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="18"/>
+    </row>
+    <row r="10" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="21" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="16"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="17"/>
-    </row>
-    <row r="11" spans="1:18" ht="15.75" customHeight="1">
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="10"/>
+    </row>
+    <row r="11" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="23"/>
-    </row>
-    <row r="12" spans="1:18" ht="15.75" customHeight="1">
+      <c r="B11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="18"/>
+    </row>
+    <row r="12" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -927,24 +938,24 @@
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
-      <c r="P12" s="20" t="s">
+      <c r="P12" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="Q12" s="19">
+      <c r="Q12" s="24">
         <f>AVERAGE(D3:P11)</f>
         <v>0.5</v>
       </c>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18" ht="15.75" customHeight="1">
+    <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="12"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="7"/>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" spans="1:18" ht="15.75" customHeight="1">
+    <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
@@ -952,7 +963,7 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" ht="15.75" customHeight="1">
+    <row r="15" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
@@ -960,7 +971,7 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" ht="15.75" customHeight="1">
+    <row r="16" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
@@ -968,7 +979,7 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="1:18" ht="15.75" customHeight="1">
+    <row r="17" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
@@ -976,7 +987,7 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="18" spans="1:18" ht="15.75" customHeight="1">
+    <row r="18" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
@@ -984,7 +995,7 @@
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
     </row>
-    <row r="19" spans="1:18" ht="15.75" customHeight="1">
+    <row r="19" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
@@ -992,7 +1003,7 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
     </row>
-    <row r="20" spans="1:18" ht="15.75" customHeight="1">
+    <row r="20" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
@@ -1000,14 +1011,14 @@
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
     </row>
-    <row r="21" spans="1:18" ht="15.75" customHeight="1">
+    <row r="21" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" spans="1:18" ht="15.75" customHeight="1">
+    <row r="22" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
@@ -1015,7 +1026,7 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
     </row>
-    <row r="23" spans="1:18" ht="15.75" customHeight="1">
+    <row r="23" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
@@ -1023,7 +1034,7 @@
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
     </row>
-    <row r="24" spans="1:18" ht="15.75" customHeight="1">
+    <row r="24" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
@@ -1031,7 +1042,7 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="1:18" ht="15.75" customHeight="1">
+    <row r="25" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
@@ -1039,7 +1050,7 @@
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
     </row>
-    <row r="26" spans="1:18" ht="15.75" customHeight="1">
+    <row r="26" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
@@ -1047,7 +1058,7 @@
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
     </row>
-    <row r="27" spans="1:18" ht="15.75" customHeight="1">
+    <row r="27" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1068,53 +1079,20 @@
     </row>
   </sheetData>
   <mergeCells count="77">
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="P6:P7"/>
-    <mergeCell ref="Q6:Q7"/>
-    <mergeCell ref="Q10:Q11"/>
-    <mergeCell ref="Q12:Q13"/>
-    <mergeCell ref="P12:P13"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="P10:P11"/>
-    <mergeCell ref="N10:N11"/>
-    <mergeCell ref="O10:O11"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="B8:C9"/>
     <mergeCell ref="B2:C3"/>
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="G6:G7"/>
@@ -1131,20 +1109,53 @@
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="B8:C9"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="Q10:Q11"/>
+    <mergeCell ref="Q12:Q13"/>
+    <mergeCell ref="P12:P13"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="P10:P11"/>
+    <mergeCell ref="N10:N11"/>
+    <mergeCell ref="O10:O11"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="Q6:Q7"/>
   </mergeCells>
   <conditionalFormatting sqref="D4:D5 E4:E7 F4:F9 G4:P11 Q4:Q13">
     <cfRule type="colorScale" priority="1">
@@ -1159,5 +1170,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>